<commit_message>
ApachePOI - excel okuma 2 GetAllData
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu4\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu5\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ApachePOI -cucumber scenario - steps -2
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,52 +63,52 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulkemb3is111</t>
-  </si>
-  <si>
-    <t>ulkemb3is122</t>
-  </si>
-  <si>
-    <t>ulkemb3is133</t>
-  </si>
-  <si>
-    <t>ulkemb3is144</t>
-  </si>
-  <si>
-    <t>ulkemb3is155</t>
-  </si>
-  <si>
-    <t>ulkemb3is166</t>
-  </si>
-  <si>
-    <t>ulkemb3is177</t>
-  </si>
-  <si>
-    <t>ulkemb3is188</t>
-  </si>
-  <si>
-    <t>ub3is111</t>
-  </si>
-  <si>
-    <t>ub3is122</t>
-  </si>
-  <si>
-    <t>ub3is133</t>
-  </si>
-  <si>
-    <t>ub3is144</t>
-  </si>
-  <si>
-    <t>ub3is155</t>
-  </si>
-  <si>
-    <t>ub3is166</t>
-  </si>
-  <si>
-    <t>ub3is177</t>
-  </si>
-  <si>
-    <t>ub3is188</t>
+    <t>ulis111</t>
+  </si>
+  <si>
+    <t>ulis112</t>
+  </si>
+  <si>
+    <t>ulis113</t>
+  </si>
+  <si>
+    <t>ulis114</t>
+  </si>
+  <si>
+    <t>ulis115</t>
+  </si>
+  <si>
+    <t>ulis116</t>
+  </si>
+  <si>
+    <t>ulis117</t>
+  </si>
+  <si>
+    <t>ulis118</t>
+  </si>
+  <si>
+    <t>ubs111</t>
+  </si>
+  <si>
+    <t>ubs112</t>
+  </si>
+  <si>
+    <t>ubs113</t>
+  </si>
+  <si>
+    <t>ubs114</t>
+  </si>
+  <si>
+    <t>ubs115</t>
+  </si>
+  <si>
+    <t>ubs116</t>
+  </si>
+  <si>
+    <t>ubs117</t>
+  </si>
+  <si>
+    <t>ubs118</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>